<commit_message>
refactoring, add async methods
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/PasswordATM.xlsx
+++ b/bin/Debug/net6.0/PasswordATM.xlsx
@@ -23,7 +23,7 @@
     </d:r>
   </si>
   <si>
-    <t>6g42qSg4dgO4oNcABTSQS1rmPWW0HoiB+PSLfAr3fEw=</t>
+    <t>hYBWtgE4/WlGEs+huGp3WEatxpS429cFBMPbA0yjjhI=</t>
   </si>
 </sst>
 </file>
@@ -86,7 +86,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" password="df50"/>
+  <sheetProtection sheet="1" password="ef1f"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactoring, implement xml for work like a database
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/PasswordATM.xlsx
+++ b/bin/Debug/net6.0/PasswordATM.xlsx
@@ -23,7 +23,7 @@
     </d:r>
   </si>
   <si>
-    <t>YHCIkLXGyh9pnHI5Fr93aAWUhTSsu/hWeBOTkSjjdfE=</t>
+    <t>5QYt8M238UtohkIIxWxADqCq8vghTn9++IErMOQ1Uws=</t>
   </si>
 </sst>
 </file>
@@ -86,7 +86,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" password="eea7"/>
+  <sheetProtection sheet="1" password="ed25"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>